<commit_message>
se agregan pequeñas correcciones en los archivos doc,pptx
</commit_message>
<xml_diff>
--- a/PROYECTO AUTO/MATERIAL AULICO/proyecto gantt.xlsx
+++ b/PROYECTO AUTO/MATERIAL AULICO/proyecto gantt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARO-FER\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Telecomunicaciones ISPC\Electronica microcontrolada\Reposotorios GitHub\Grupo3\PROYECTO AUTO\MATERIAL AULICO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C1435F-5843-4E94-A789-36387E3DD276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA0EEEF-CF10-4A57-B98B-D33E46D88DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="15576" windowHeight="8832" xr2:uid="{C86992EC-E09A-43DB-9A47-8CB92B7AC45C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C86992EC-E09A-43DB-9A47-8CB92B7AC45C}"/>
   </bookViews>
   <sheets>
     <sheet name="GANTT GRUPO 1" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd\-mm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -194,14 +194,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
@@ -534,7 +534,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="446811784"/>
@@ -608,7 +608,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="555510888"/>
@@ -654,7 +654,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1550,20 +1550,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62532BA5-07BF-403F-9520-5ECFEB36E4DD}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>44816</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>44811</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>44814</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>44821</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>44816</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>44818</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>44818</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>44822</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>44818</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>44822</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>44827</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>44809</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>